<commit_message>
Professional status: distinguish employees and self-employed, exclude family workers
Prepare dataset for reg
</commit_message>
<xml_diff>
--- a/Tables/LFS_missing_weights.xlsx
+++ b/Tables/LFS_missing_weights.xlsx
@@ -391,16 +391,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>13.63508621117216</v>
+        <v>13.62512651192116</v>
       </c>
       <c r="C2">
-        <v>14.02697559509919</v>
+        <v>14.01869158878505</v>
       </c>
       <c r="D2">
-        <v>14.40656241989305</v>
+        <v>14.41015089163237</v>
       </c>
       <c r="E2">
-        <v>13.5751255161198</v>
+        <v>13.58103904184166</v>
       </c>
     </row>
     <row r="3">
@@ -410,13 +410,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>5.966378145794531</v>
+        <v>5.966137459807074</v>
       </c>
       <c r="C3">
-        <v>7.189622021563845</v>
+        <v>7.184048480109471</v>
       </c>
       <c r="D3">
-        <v>2.555976933866669</v>
+        <v>2.547654436882318</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -429,16 +429,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>48.2007188025993</v>
+        <v>48.21894005212858</v>
       </c>
       <c r="C4">
-        <v>48.01018047201264</v>
+        <v>47.99981415230219</v>
       </c>
       <c r="D4">
-        <v>47.26901976016627</v>
+        <v>47.28610407328006</v>
       </c>
       <c r="E4">
-        <v>45.69394272550695</v>
+        <v>45.65205927332173</v>
       </c>
     </row>
     <row r="5">
@@ -457,7 +457,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>49.68832640725541</v>
+        <v>49.76771196283391</v>
       </c>
     </row>
     <row r="6">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>43.4740750928318</v>
+        <v>43.42524594706942</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -495,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>55.61030444969467</v>
+        <v>55.54603894698204</v>
       </c>
     </row>
     <row r="8">
@@ -505,16 +505,16 @@
         </is>
       </c>
       <c r="B8">
-        <v>2.529787999889176</v>
+        <v>2.527362816151457</v>
       </c>
       <c r="C8">
-        <v>3.390499830756927</v>
+        <v>3.379581225804629</v>
       </c>
       <c r="D8">
-        <v>3.63371194799107</v>
+        <v>3.621518485479235</v>
       </c>
       <c r="E8">
-        <v>4.736614091105729</v>
+        <v>4.730001771536243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many new descriptive tables, uniformed nomenclature
New/improved tables (most are companions to existing figures):
- Telework_NUTS
- Telework_degurba
- Telework_stapro
- Telework_work_location
- Telework_intentisty_country_nuts

Aggregate variable is now everywhere
telework_share = weighted.mean(homework_any, wt = coeffy)
and labelled "Share of people teleworking"
</commit_message>
<xml_diff>
--- a/Tables/LFS_missing_weights.xlsx
+++ b/Tables/LFS_missing_weights.xlsx
@@ -391,16 +391,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>13.62512651192116</v>
+        <v>13.62512651191992</v>
       </c>
       <c r="C2">
-        <v>14.01869158878505</v>
+        <v>14.01869158878591</v>
       </c>
       <c r="D2">
-        <v>14.41015089163237</v>
+        <v>14.41015089163176</v>
       </c>
       <c r="E2">
-        <v>13.58103904184166</v>
+        <v>13.58103904184097</v>
       </c>
     </row>
     <row r="3">
@@ -410,13 +410,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>5.966137459807074</v>
+        <v>5.966137459806931</v>
       </c>
       <c r="C3">
-        <v>7.184048480109471</v>
+        <v>7.184048480109167</v>
       </c>
       <c r="D3">
-        <v>2.547654436882318</v>
+        <v>2.547654436882271</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -429,16 +429,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>48.21894005212858</v>
+        <v>48.21894005213944</v>
       </c>
       <c r="C4">
-        <v>47.99981415230219</v>
+        <v>47.9998141522948</v>
       </c>
       <c r="D4">
-        <v>47.28610407328006</v>
+        <v>47.28610407328582</v>
       </c>
       <c r="E4">
-        <v>45.65205927332173</v>
+        <v>45.65205927331449</v>
       </c>
     </row>
     <row r="5">
@@ -457,7 +457,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>49.76771196283391</v>
+        <v>49.76771196282979</v>
       </c>
     </row>
     <row r="6">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>43.42524594706942</v>
+        <v>43.42524594706785</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -495,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>55.54603894698204</v>
+        <v>55.54603894701359</v>
       </c>
     </row>
     <row r="8">
@@ -505,16 +505,16 @@
         </is>
       </c>
       <c r="B8">
-        <v>2.527362816151457</v>
+        <v>2.527362816151617</v>
       </c>
       <c r="C8">
-        <v>3.379581225804629</v>
+        <v>3.37958122580461</v>
       </c>
       <c r="D8">
-        <v>3.621518485479235</v>
+        <v>3.621518485479176</v>
       </c>
       <c r="E8">
-        <v>4.730001771536243</v>
+        <v>4.730001771536375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated descriptives to new data
- 2022 LFS
- 2019:2023 connectivity data
- experiment with sector statistics
</commit_message>
<xml_diff>
--- a/Tables/LFS_missing_weights.xlsx
+++ b/Tables/LFS_missing_weights.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -383,6 +383,11 @@
           <t>2021</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -391,16 +396,19 @@
         </is>
       </c>
       <c r="B2">
-        <v>13.62512651191992</v>
+        <v>13.62512651192116</v>
       </c>
       <c r="C2">
-        <v>14.01869158878591</v>
+        <v>14.01869158878505</v>
       </c>
       <c r="D2">
-        <v>14.41015089163176</v>
+        <v>14.41015089163237</v>
       </c>
       <c r="E2">
-        <v>13.58103904184097</v>
+        <v>13.58607951783805</v>
+      </c>
+      <c r="F2">
+        <v>13.75910054372869</v>
       </c>
     </row>
     <row r="3">
@@ -410,15 +418,18 @@
         </is>
       </c>
       <c r="B3">
-        <v>5.966137459806931</v>
+        <v>5.966137459807074</v>
       </c>
       <c r="C3">
-        <v>7.184048480109167</v>
+        <v>7.184048480109471</v>
       </c>
       <c r="D3">
-        <v>2.547654436882271</v>
+        <v>2.547654436882318</v>
       </c>
       <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
     </row>
@@ -429,16 +440,19 @@
         </is>
       </c>
       <c r="B4">
-        <v>48.21894005213944</v>
+        <v>48.21894005212858</v>
       </c>
       <c r="C4">
-        <v>47.9998141522948</v>
+        <v>47.99981415230219</v>
       </c>
       <c r="D4">
-        <v>47.28610407328582</v>
+        <v>47.28610407328006</v>
       </c>
       <c r="E4">
-        <v>45.65205927331449</v>
+        <v>45.65205927332173</v>
+      </c>
+      <c r="F4">
+        <v>45.37589150005846</v>
       </c>
     </row>
     <row r="5">
@@ -457,7 +471,10 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>49.76771196282979</v>
+        <v>49.76771196283391</v>
+      </c>
+      <c r="F5">
+        <v>49.83548766157461</v>
       </c>
     </row>
     <row r="6">
@@ -467,7 +484,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>43.42524594706785</v>
+        <v>43.42524594706942</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -476,6 +493,9 @@
         <v>0</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>0</v>
       </c>
     </row>
@@ -495,7 +515,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>55.54603894701359</v>
+        <v>54.95245452898037</v>
+      </c>
+      <c r="F7">
+        <v>60.73966448725332</v>
       </c>
     </row>
     <row r="8">
@@ -505,16 +528,19 @@
         </is>
       </c>
       <c r="B8">
-        <v>2.527362816151617</v>
+        <v>2.527362816151457</v>
       </c>
       <c r="C8">
-        <v>3.37958122580461</v>
+        <v>3.379581225804629</v>
       </c>
       <c r="D8">
-        <v>3.621518485479176</v>
+        <v>3.621518485479235</v>
       </c>
       <c r="E8">
-        <v>4.730001771536375</v>
+        <v>4.730001771536243</v>
+      </c>
+      <c r="F8">
+        <v>5.931610986514432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>